<commit_message>
Naming undirected and renaming directed to none
</commit_message>
<xml_diff>
--- a/mtsim/examples/network_2.xlsx
+++ b/mtsim/examples/network_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,7 @@
     <sheet name="links" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">links!$B$1:$B$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">links!$B$1:$B$84</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -159,6 +159,12 @@
     <t xml:space="preserve">BB</t>
   </si>
   <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">qmax</t>
   </si>
   <si>
@@ -198,10 +204,7 @@
     <t xml:space="preserve">node_to</t>
   </si>
   <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l</t>
+    <t xml:space="preserve">length</t>
   </si>
   <si>
     <t xml:space="preserve">count</t>
@@ -274,17 +277,19 @@
   </si>
   <si>
     <t xml:space="preserve">Hybe-BB I/72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conn BA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -306,6 +311,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,7 +367,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,19 +390,19 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -422,7 +434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -434,7 +446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -446,7 +458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -458,7 +470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -470,7 +482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -482,7 +494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -494,7 +506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -506,7 +518,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -518,7 +530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -530,7 +542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -542,7 +554,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -554,7 +566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -566,7 +578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -578,7 +590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
@@ -590,7 +602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -602,7 +614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -614,7 +626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -626,7 +638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -638,7 +650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
@@ -650,7 +662,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
@@ -662,7 +674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -674,7 +686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
@@ -694,6 +706,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C24" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="D24" s="0" t="s">
         <v>32</v>
       </c>
@@ -707,10 +722,10 @@
       <c r="G24" s="0" t="n">
         <v>205260</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="0" t="n">
         <v>452963</v>
       </c>
-      <c r="I24" s="1" t="n">
+      <c r="I24" s="0" t="n">
         <v>7376</v>
       </c>
       <c r="J24" s="0" t="n">
@@ -725,6 +740,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C25" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="0" t="s">
         <v>33</v>
       </c>
@@ -738,10 +756,10 @@
       <c r="G25" s="0" t="n">
         <v>57249</v>
       </c>
-      <c r="H25" s="1" t="n">
+      <c r="H25" s="0" t="n">
         <v>59767</v>
       </c>
-      <c r="I25" s="1" t="n">
+      <c r="I25" s="0" t="n">
         <v>3283</v>
       </c>
       <c r="J25" s="0" t="n">
@@ -756,6 +774,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C26" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="D26" s="0" t="s">
         <v>34</v>
       </c>
@@ -769,10 +790,10 @@
       <c r="G26" s="0" t="n">
         <v>57884</v>
       </c>
-      <c r="H26" s="1" t="n">
+      <c r="H26" s="0" t="n">
         <v>69682</v>
       </c>
-      <c r="I26" s="1" t="n">
+      <c r="I26" s="0" t="n">
         <v>3307</v>
       </c>
       <c r="J26" s="0" t="n">
@@ -787,6 +808,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C27" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="D27" s="0" t="s">
         <v>35</v>
       </c>
@@ -800,10 +824,10 @@
       <c r="G27" s="0" t="n">
         <v>48090</v>
       </c>
-      <c r="H27" s="1" t="n">
+      <c r="H27" s="0" t="n">
         <v>46862</v>
       </c>
-      <c r="I27" s="1" t="n">
+      <c r="I27" s="0" t="n">
         <v>2613</v>
       </c>
       <c r="J27" s="0" t="n">
@@ -818,6 +842,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C28" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="D28" s="0" t="s">
         <v>36</v>
       </c>
@@ -831,10 +858,10 @@
       <c r="G28" s="0" t="n">
         <v>59621</v>
       </c>
-      <c r="H28" s="1" t="n">
+      <c r="H28" s="0" t="n">
         <v>76939</v>
       </c>
-      <c r="I28" s="1" t="n">
+      <c r="I28" s="0" t="n">
         <v>3361</v>
       </c>
       <c r="J28" s="0" t="n">
@@ -849,6 +876,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C29" s="0" t="s">
+        <v>37</v>
+      </c>
       <c r="D29" s="0" t="s">
         <v>37</v>
       </c>
@@ -862,10 +892,10 @@
       <c r="G29" s="0" t="n">
         <v>39496</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="0" t="n">
         <v>36090</v>
       </c>
-      <c r="I29" s="1" t="n">
+      <c r="I29" s="0" t="n">
         <v>2110</v>
       </c>
       <c r="J29" s="0" t="n">
@@ -880,6 +910,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C30" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="D30" s="0" t="s">
         <v>38</v>
       </c>
@@ -893,10 +926,10 @@
       <c r="G30" s="0" t="n">
         <v>21636</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="0" t="n">
         <v>17855</v>
       </c>
-      <c r="I30" s="1" t="n">
+      <c r="I30" s="0" t="n">
         <v>1593</v>
       </c>
       <c r="J30" s="0" t="n">
@@ -911,6 +944,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C31" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="D31" s="0" t="s">
         <v>39</v>
       </c>
@@ -924,10 +960,10 @@
       <c r="G31" s="0" t="n">
         <v>34308</v>
       </c>
-      <c r="H31" s="1" t="n">
+      <c r="H31" s="0" t="n">
         <v>35694</v>
       </c>
-      <c r="I31" s="1" t="n">
+      <c r="I31" s="0" t="n">
         <v>2169</v>
       </c>
       <c r="J31" s="0" t="n">
@@ -942,6 +978,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C32" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="D32" s="0" t="s">
         <v>40</v>
       </c>
@@ -955,10 +994,10 @@
       <c r="G32" s="0" t="n">
         <v>51148</v>
       </c>
-      <c r="H32" s="1" t="n">
+      <c r="H32" s="0" t="n">
         <v>59491</v>
       </c>
-      <c r="I32" s="1" t="n">
+      <c r="I32" s="0" t="n">
         <v>3768</v>
       </c>
       <c r="J32" s="0" t="n">
@@ -973,6 +1012,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C33" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="D33" s="0" t="s">
         <v>41</v>
       </c>
@@ -986,10 +1028,10 @@
       <c r="G33" s="0" t="n">
         <v>88023</v>
       </c>
-      <c r="H33" s="1" t="n">
+      <c r="H33" s="0" t="n">
         <v>127412</v>
       </c>
-      <c r="I33" s="1" t="n">
+      <c r="I33" s="0" t="n">
         <v>4657</v>
       </c>
       <c r="J33" s="0" t="n">
@@ -1004,6 +1046,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C34" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="D34" s="0" t="s">
         <v>42</v>
       </c>
@@ -1017,10 +1062,10 @@
       <c r="G34" s="0" t="n">
         <v>27599</v>
       </c>
-      <c r="H34" s="1" t="n">
+      <c r="H34" s="0" t="n">
         <v>27293</v>
       </c>
-      <c r="I34" s="1" t="n">
+      <c r="I34" s="0" t="n">
         <v>1648</v>
       </c>
       <c r="J34" s="0" t="n">
@@ -1035,6 +1080,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="C35" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="D35" s="0" t="s">
         <v>43</v>
       </c>
@@ -1048,10 +1096,10 @@
       <c r="G35" s="0" t="n">
         <v>40193</v>
       </c>
-      <c r="H35" s="1" t="n">
+      <c r="H35" s="0" t="n">
         <v>48863</v>
       </c>
-      <c r="I35" s="1" t="n">
+      <c r="I35" s="0" t="n">
         <v>2119</v>
       </c>
       <c r="J35" s="0" t="n">
@@ -1076,30 +1124,30 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,10 +1155,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>70000</v>
+        <v>35000</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>110</v>
@@ -1127,10 +1175,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>125</v>
@@ -1147,10 +1195,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>90</v>
@@ -1167,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>80</v>
@@ -1187,10 +1235,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>15000</v>
+        <v>7500</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>65</v>
@@ -1207,10 +1255,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>15000</v>
+        <v>7500</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>50</v>
@@ -1227,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>40</v>
@@ -1258,19 +1306,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1279,22 +1326,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,844 +1361,1708 @@
         <v>36</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>45085</v>
+        <v>22543</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>36.006</v>
+        <v>36</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>61</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>25135</v>
+        <v>22543</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>75.005</v>
+        <v>36.006</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>19088</v>
+        <v>12568</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>71.69</v>
+        <v>36.006</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>17280</v>
+        <v>12568</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>24.33</v>
+        <v>75.005</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>20196</v>
+        <v>9544</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>33.954</v>
+        <v>75.005</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>12467</v>
+        <v>9544</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>7.597</v>
+        <v>71.69</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>17804</v>
+        <v>8640</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>69.921</v>
+        <v>71.69</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>8170</v>
+        <v>8640</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>2.366</v>
+        <v>24.33</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>20740</v>
+        <v>10098</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>4.702</v>
+        <v>24.33</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>14755</v>
+        <v>10098</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>28.518</v>
+        <v>33.954</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>15729</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>11.595</v>
+        <v>33.954</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>13117</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>87.491</v>
+        <v>7.597</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>17395</v>
+        <v>8902</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>5.349</v>
+        <v>7.597</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>13985</v>
+        <v>8902</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>14.296</v>
+        <v>69.921</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>21584</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>2.375</v>
+        <v>69.921</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>25662</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>4.59</v>
+        <v>2.366</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>11592</v>
+        <v>10370</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>7.123</v>
+        <v>2.366</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>14629</v>
+        <v>10370</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>48.731</v>
+        <v>4.702</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>7699</v>
+        <v>7378</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>191.308</v>
+        <v>4.702</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>7166</v>
+        <v>7378</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C22" s="0" t="n">
-        <v>14</v>
-      </c>
       <c r="D22" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>8.233</v>
+        <v>28.518</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>30427</v>
+        <v>7865</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>40.261</v>
+        <v>28.518</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>11091</v>
+        <v>7865</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>29.173</v>
+        <v>11.595</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>11922</v>
+        <v>6559</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>67.4</v>
+        <v>11.595</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>2719</v>
+        <v>6559</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>10.036</v>
+        <v>87.491</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>8698</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>5</v>
+        <v>87.491</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>8698</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>6</v>
+        <v>5.349</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>6993</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>3.649</v>
+        <v>5.349</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>6993</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>5</v>
+        <v>14.296</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>10792</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>2.09</v>
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>14.296</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>10792</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>2.688</v>
+        <v>2.375</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>12831</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>0.822</v>
+        <v>2.375</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>12831</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>2.771</v>
+        <v>4.59</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>5796</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>1.046</v>
+        <v>4.59</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>5796</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>110</v>
+        <v>18</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>2.588</v>
+        <v>7.123</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>7315</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>2.703</v>
+        <v>7.123</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>7315</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>112</v>
+        <v>19</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>2.809</v>
+        <v>48.731</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>3850</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>4.037</v>
+        <v>48.731</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>3850</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>2.954</v>
+        <v>191.308</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>3583</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>1.385</v>
+        <v>191.308</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>3583</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>1.502</v>
+        <v>8.233</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>15214</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>8.233</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>15214</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>40.261</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>5546</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>40.261</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>5546</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>29.173</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>5961</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>29.173</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>5961</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>67.4</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>67.4</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>10.036</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>10.036</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>3.649</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>3.649</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>2.688</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>2.688</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>0.822</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>0.822</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>2.771</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>2.771</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>1.046</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>1.046</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>2.588</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>2.588</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>2.703</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>2.703</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>2.809</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>2.809</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>4.037</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>4.037</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>2.954</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>2.954</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>1.385</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1.385</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1.502</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>1.502</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
         <v>117</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B84" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C84" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="D43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="0" t="n">
+      <c r="D84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>3.652</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="0" t="n">
         <v>3.652</v>
       </c>
     </row>

</xml_diff>